<commit_message>
fix extraneous header row
</commit_message>
<xml_diff>
--- a/Data Test (xlsx).xlsx
+++ b/Data Test (xlsx).xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
-  <si>
-    <t>Stocks Test (no unique) - stocks (5)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Stocks</t>
   </si>
@@ -59,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -71,13 +68,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,8 +98,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -210,41 +218,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -268,15 +387,17 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Blank">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -284,28 +405,28 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="00A2FF"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="16E7CF"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="61D836"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFD932"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF644E"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="FF42A1"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -314,7 +435,7 @@
         <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Blank">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Helvetica Neue"/>
         <a:ea typeface="Helvetica Neue"/>
@@ -326,7 +447,7 @@
         <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Blank">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -405,7 +526,13 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -464,47 +591,50 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Cambria"/>
+            <a:ea typeface="Cambria"/>
+            <a:cs typeface="Cambria"/>
+            <a:sym typeface="Cambria"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -752,14 +882,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1044,38 +1180,38 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Cambria"/>
+            <a:ea typeface="Cambria"/>
+            <a:cs typeface="Cambria"/>
+            <a:sym typeface="Cambria"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1329,11 +1465,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.67188" style="1" customWidth="1"/>
@@ -1341,155 +1477,180 @@
     <col min="4" max="6" width="5" style="1" customWidth="1"/>
     <col min="7" max="7" width="4" style="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="3">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="3">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s" s="3">
         <v>8</v>
       </c>
+      <c r="B2" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.91</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.08</v>
+      </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="B3" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0.91</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="B3" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="D3" s="8">
         <v>0.15</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="8">
         <v>0.1</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="8">
         <v>0.13</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="8">
         <v>0.07000000000000001</v>
       </c>
-      <c r="H3" s="6">
-        <v>0.08</v>
+      <c r="H3" s="8">
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="A4" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>0.3</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>0.25</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
+        <v>0.13</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="8">
         <v>0.15</v>
       </c>
-      <c r="E4" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0.13</v>
-      </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>0.07000000000000001</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="A5" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="B5" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="B5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="D5" s="8">
         <v>0.13</v>
       </c>
-      <c r="E5" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="E5" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="F5" s="8">
         <v>0.15</v>
       </c>
-      <c r="G5" s="9">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="H5" s="9">
-        <v>0.07000000000000001</v>
+      <c r="G5" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.19</v>
       </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0.24</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0.13</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0.11</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="G6" s="9">
-        <v>0.09</v>
-      </c>
-      <c r="H6" s="9">
-        <v>0.19</v>
-      </c>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>